<commit_message>
Add Python compatibility inspection setting, extend README with development setup and backend instructions, and enhance index.html content
- Introduced PythonCompatibilityInspectionAdvertiser configuration in `.idea/misc.xml`.
- Expanded README with detailed steps for setting up development environment, running server scripts, importing data from Excel/PDF, and database operations.
- Updated `index.html` to include new content sections, backend templates, and documentation links.
- Added `.flake8` file to configure style rules; ignored specific checks already addressed by Black.
- Included `error.txt` for inspection results and diagnostic references.

Signed-off-by: Your Name <you@example.com>
</commit_message>
<xml_diff>
--- a/DOC/school_DATA/students_03.xlsx
+++ b/DOC/school_DATA/students_03.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sh_shool_011\DOC\school_DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sh_school_015\DOC\school_DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16439F3-ED41-431D-9AD4-0CED3DCE8996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C5B078-4D42-420E-A37B-0B4DF3D5122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="33749" windowHeight="20474" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6940,7 +6940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C150" sqref="C150"/>
     </sheetView>
   </sheetViews>
@@ -6948,7 +6948,7 @@
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.375" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>

</xml_diff>